<commit_message>
1. Added the appendix. 2. Change some names of the variables. 3. Finished the paper. (Results and Conclusion, Abstract).
Undone: nomenclature.
</commit_message>
<xml_diff>
--- a/SolarThermalDesign/Water/ResultAnalysis/P_VS_C.xlsx
+++ b/SolarThermalDesign/Water/ResultAnalysis/P_VS_C.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="20295" windowHeight="9735" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="20295" windowHeight="9735"/>
   </bookViews>
   <sheets>
     <sheet name="Parallelflow" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="16">
   <si>
     <t>T_1_i[i]</t>
   </si>
@@ -51,6 +51,26 @@
   </si>
   <si>
     <t>Power</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>eta_stirlingEngine[]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T_2_o[x]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T_2_i[x]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T_1_o[x]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T_1_i[x]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -173,34 +193,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1073</c:v>
+                  <c:v>1073.1500000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1023</c:v>
+                  <c:v>1022.38</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>975.3</c:v>
+                  <c:v>974.35</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>931</c:v>
+                  <c:v>928.9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>889.5</c:v>
+                  <c:v>885.91</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>850.5</c:v>
+                  <c:v>845.26</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>814</c:v>
+                  <c:v>806.82</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>779.8</c:v>
+                  <c:v>770.49</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>747.7</c:v>
+                  <c:v>736.16</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>717.6</c:v>
+                  <c:v>703.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -255,34 +275,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1023</c:v>
+                  <c:v>327.17</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>975.3</c:v>
+                  <c:v>329.8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>931</c:v>
+                  <c:v>332.29</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>889.5</c:v>
+                  <c:v>334.65</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>850.5</c:v>
+                  <c:v>336.88</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>814</c:v>
+                  <c:v>339</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>779.8</c:v>
+                  <c:v>341.01</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>747.7</c:v>
+                  <c:v>342.91</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>717.6</c:v>
+                  <c:v>344.71</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>689.4</c:v>
+                  <c:v>346.43</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -337,34 +357,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>327</c:v>
+                  <c:v>1022</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>341.3</c:v>
+                  <c:v>974.3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>354.8</c:v>
+                  <c:v>928.9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>367.4</c:v>
+                  <c:v>885.9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>379.4</c:v>
+                  <c:v>845.3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>390.6</c:v>
+                  <c:v>806.8</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>401.3</c:v>
+                  <c:v>770.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>411.3</c:v>
+                  <c:v>736.2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>420.8</c:v>
+                  <c:v>703.7</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>429.8</c:v>
+                  <c:v>673.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -419,34 +439,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>341.3</c:v>
+                  <c:v>329.8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>354.8</c:v>
+                  <c:v>332.3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>367.4</c:v>
+                  <c:v>334.7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>379.4</c:v>
+                  <c:v>336.9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>390.6</c:v>
+                  <c:v>339</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>401.3</c:v>
+                  <c:v>341</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>411.3</c:v>
+                  <c:v>342.9</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>420.8</c:v>
+                  <c:v>344.7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>429.8</c:v>
+                  <c:v>346.4</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>438.4</c:v>
+                  <c:v>348.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -501,34 +521,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>969.9</c:v>
+                  <c:v>0.36480000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>926</c:v>
+                  <c:v>0.3599</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>884.8</c:v>
+                  <c:v>0.35439999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>846.1</c:v>
+                  <c:v>0.34849999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>809.9</c:v>
+                  <c:v>0.34189999999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>775.9</c:v>
+                  <c:v>0.3347</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>744</c:v>
+                  <c:v>0.32690000000000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>714.2</c:v>
+                  <c:v>0.31840000000000002</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>686.2</c:v>
+                  <c:v>0.309</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>660</c:v>
+                  <c:v>0.2989</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -582,36 +602,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>345.4</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>358.6</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>371.1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>382.8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>393.8</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>404.3</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>414.2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>423.5</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>432.4</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>440.9</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -664,57 +654,27 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>604.9</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>598.1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>591.20000000000005</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>584.1</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>577.1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>570</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>563.1</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>556.29999999999995</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>549.6</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>543.1</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="62027264"/>
-        <c:axId val="62025728"/>
+        <c:axId val="87911424"/>
+        <c:axId val="94057600"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="62027264"/>
+        <c:axId val="87911424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62025728"/>
+        <c:crossAx val="94057600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="62025728"/>
+        <c:axId val="94057600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="300"/>
@@ -723,7 +683,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62027264"/>
+        <c:crossAx val="87911424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -736,7 +696,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1324,23 +1284,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="97557504"/>
-        <c:axId val="97563392"/>
+        <c:axId val="94090752"/>
+        <c:axId val="94092288"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="97557504"/>
+        <c:axId val="94090752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97563392"/>
+        <c:crossAx val="94092288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="97563392"/>
+        <c:axId val="94092288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="300"/>
@@ -1349,7 +1309,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97557504"/>
+        <c:crossAx val="94090752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1362,7 +1322,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1680,23 +1640,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="45147648"/>
-        <c:axId val="45146112"/>
+        <c:axId val="94155904"/>
+        <c:axId val="94157440"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="45147648"/>
+        <c:axId val="94155904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45146112"/>
+        <c:crossAx val="94157440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="45146112"/>
+        <c:axId val="94157440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1704,7 +1664,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45147648"/>
+        <c:crossAx val="94155904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1717,7 +1677,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2029,23 +1989,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="95496064"/>
-        <c:axId val="93453312"/>
+        <c:axId val="94173824"/>
+        <c:axId val="94962048"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="95496064"/>
+        <c:axId val="94173824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93453312"/>
+        <c:crossAx val="94962048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="93453312"/>
+        <c:axId val="94962048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2053,7 +2013,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95496064"/>
+        <c:crossAx val="94173824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2066,7 +2026,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2076,16 +2036,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>647700</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2494,27 +2454,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:H12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="B1" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="G1" t="s">
         <v>5</v>
@@ -2551,25 +2511,19 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>1073</v>
+        <v>1073.1500000000001</v>
       </c>
       <c r="C3">
-        <v>1023</v>
+        <v>327.17</v>
       </c>
       <c r="D3">
-        <v>327</v>
+        <v>1022</v>
       </c>
       <c r="E3">
-        <v>341.3</v>
+        <v>329.8</v>
       </c>
       <c r="F3">
-        <v>969.9</v>
-      </c>
-      <c r="G3">
-        <v>345.4</v>
-      </c>
-      <c r="H3">
-        <v>604.9</v>
+        <v>0.36480000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -2577,25 +2531,19 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>1023</v>
+        <v>1022.38</v>
       </c>
       <c r="C4">
-        <v>975.3</v>
+        <v>329.8</v>
       </c>
       <c r="D4">
-        <v>341.3</v>
+        <v>974.3</v>
       </c>
       <c r="E4">
-        <v>354.8</v>
+        <v>332.3</v>
       </c>
       <c r="F4">
-        <v>926</v>
-      </c>
-      <c r="G4">
-        <v>358.6</v>
-      </c>
-      <c r="H4">
-        <v>598.1</v>
+        <v>0.3599</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -2603,25 +2551,19 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>975.3</v>
+        <v>974.35</v>
       </c>
       <c r="C5">
-        <v>931</v>
+        <v>332.29</v>
       </c>
       <c r="D5">
-        <v>354.8</v>
+        <v>928.9</v>
       </c>
       <c r="E5">
-        <v>367.4</v>
+        <v>334.7</v>
       </c>
       <c r="F5">
-        <v>884.8</v>
-      </c>
-      <c r="G5">
-        <v>371.1</v>
-      </c>
-      <c r="H5">
-        <v>591.20000000000005</v>
+        <v>0.35439999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -2629,25 +2571,19 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>931</v>
+        <v>928.9</v>
       </c>
       <c r="C6">
-        <v>889.5</v>
+        <v>334.65</v>
       </c>
       <c r="D6">
-        <v>367.4</v>
+        <v>885.9</v>
       </c>
       <c r="E6">
-        <v>379.4</v>
+        <v>336.9</v>
       </c>
       <c r="F6">
-        <v>846.1</v>
-      </c>
-      <c r="G6">
-        <v>382.8</v>
-      </c>
-      <c r="H6">
-        <v>584.1</v>
+        <v>0.34849999999999998</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -2655,25 +2591,19 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>889.5</v>
+        <v>885.91</v>
       </c>
       <c r="C7">
-        <v>850.5</v>
+        <v>336.88</v>
       </c>
       <c r="D7">
-        <v>379.4</v>
+        <v>845.3</v>
       </c>
       <c r="E7">
-        <v>390.6</v>
+        <v>339</v>
       </c>
       <c r="F7">
-        <v>809.9</v>
-      </c>
-      <c r="G7">
-        <v>393.8</v>
-      </c>
-      <c r="H7">
-        <v>577.1</v>
+        <v>0.34189999999999998</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -2681,25 +2611,19 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>850.5</v>
+        <v>845.26</v>
       </c>
       <c r="C8">
-        <v>814</v>
+        <v>339</v>
       </c>
       <c r="D8">
-        <v>390.6</v>
+        <v>806.8</v>
       </c>
       <c r="E8">
-        <v>401.3</v>
+        <v>341</v>
       </c>
       <c r="F8">
-        <v>775.9</v>
-      </c>
-      <c r="G8">
-        <v>404.3</v>
-      </c>
-      <c r="H8">
-        <v>570</v>
+        <v>0.3347</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -2707,25 +2631,19 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>814</v>
+        <v>806.82</v>
       </c>
       <c r="C9">
-        <v>779.8</v>
+        <v>341.01</v>
       </c>
       <c r="D9">
-        <v>401.3</v>
+        <v>770.5</v>
       </c>
       <c r="E9">
-        <v>411.3</v>
+        <v>342.9</v>
       </c>
       <c r="F9">
-        <v>744</v>
-      </c>
-      <c r="G9">
-        <v>414.2</v>
-      </c>
-      <c r="H9">
-        <v>563.1</v>
+        <v>0.32690000000000002</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -2733,25 +2651,19 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>779.8</v>
+        <v>770.49</v>
       </c>
       <c r="C10">
-        <v>747.7</v>
+        <v>342.91</v>
       </c>
       <c r="D10">
-        <v>411.3</v>
+        <v>736.2</v>
       </c>
       <c r="E10">
-        <v>420.8</v>
+        <v>344.7</v>
       </c>
       <c r="F10">
-        <v>714.2</v>
-      </c>
-      <c r="G10">
-        <v>423.5</v>
-      </c>
-      <c r="H10">
-        <v>556.29999999999995</v>
+        <v>0.31840000000000002</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -2759,25 +2671,19 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>747.7</v>
+        <v>736.16</v>
       </c>
       <c r="C11">
-        <v>717.6</v>
+        <v>344.71</v>
       </c>
       <c r="D11">
-        <v>420.8</v>
+        <v>703.7</v>
       </c>
       <c r="E11">
-        <v>429.8</v>
+        <v>346.4</v>
       </c>
       <c r="F11">
-        <v>686.2</v>
-      </c>
-      <c r="G11">
-        <v>432.4</v>
-      </c>
-      <c r="H11">
-        <v>549.6</v>
+        <v>0.309</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -2785,25 +2691,19 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>717.6</v>
+        <v>703.75</v>
       </c>
       <c r="C12">
-        <v>689.4</v>
+        <v>346.43</v>
       </c>
       <c r="D12">
-        <v>429.8</v>
+        <v>673.1</v>
       </c>
       <c r="E12">
-        <v>438.4</v>
+        <v>348.1</v>
       </c>
       <c r="F12">
-        <v>660</v>
-      </c>
-      <c r="G12">
-        <v>440.9</v>
-      </c>
-      <c r="H12">
-        <v>543.1</v>
+        <v>0.2989</v>
       </c>
     </row>
   </sheetData>
@@ -3140,7 +3040,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2:G21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Tiny changes made of the TeX file.
</commit_message>
<xml_diff>
--- a/SolarThermalDesign/Water/ResultAnalysis/P_VS_C.xlsx
+++ b/SolarThermalDesign/Water/ResultAnalysis/P_VS_C.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="20295" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="20295" windowHeight="9735" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Parallelflow" sheetId="1" r:id="rId1"/>
@@ -658,23 +658,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="87911424"/>
-        <c:axId val="94057600"/>
+        <c:axId val="102174080"/>
+        <c:axId val="102188160"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="87911424"/>
+        <c:axId val="102174080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94057600"/>
+        <c:crossAx val="102188160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="94057600"/>
+        <c:axId val="102188160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="300"/>
@@ -683,7 +683,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87911424"/>
+        <c:crossAx val="102174080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -696,7 +696,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1284,23 +1284,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="94090752"/>
-        <c:axId val="94092288"/>
+        <c:axId val="102532608"/>
+        <c:axId val="102534144"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="94090752"/>
+        <c:axId val="102532608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94092288"/>
+        <c:crossAx val="102534144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="94092288"/>
+        <c:axId val="102534144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="300"/>
@@ -1309,7 +1309,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94090752"/>
+        <c:crossAx val="102532608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1322,7 +1322,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1480,7 +1480,7 @@
                 <c:pt idx="19">
                   <c:v>0.34031699999999998</c:v>
                 </c:pt>
-                <c:pt idx="20" formatCode="0.00E+00">
+                <c:pt idx="20">
                   <c:v>0.34045799999999998</c:v>
                 </c:pt>
               </c:numCache>
@@ -1632,7 +1632,7 @@
                 <c:pt idx="19">
                   <c:v>0.34115400000000001</c:v>
                 </c:pt>
-                <c:pt idx="20" formatCode="0.00E+00">
+                <c:pt idx="20">
                   <c:v>0.34126200000000001</c:v>
                 </c:pt>
               </c:numCache>
@@ -1640,23 +1640,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="94155904"/>
-        <c:axId val="94157440"/>
+        <c:axId val="91755648"/>
+        <c:axId val="91757184"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="94155904"/>
+        <c:axId val="91755648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94157440"/>
+        <c:crossAx val="91757184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="94157440"/>
+        <c:axId val="91757184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1664,20 +1664,16 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94155904"/>
+        <c:crossAx val="91755648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1989,23 +1985,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="94173824"/>
-        <c:axId val="94962048"/>
+        <c:axId val="91781760"/>
+        <c:axId val="91787648"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="94173824"/>
+        <c:axId val="91781760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94962048"/>
+        <c:crossAx val="91787648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="94962048"/>
+        <c:axId val="91787648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2013,7 +2009,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94173824"/>
+        <c:crossAx val="91781760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2026,7 +2022,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2106,16 +2102,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2454,7 +2450,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3:F12"/>
     </sheetView>
   </sheetViews>
@@ -3040,8 +3036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:G22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:G21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -3427,10 +3423,10 @@
       <c r="B22" s="2">
         <v>10</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C22" s="2">
         <v>0.34045799999999998</v>
       </c>
-      <c r="D22" s="1">
+      <c r="D22" s="2">
         <v>0.34126200000000001</v>
       </c>
       <c r="F22" s="1">

</xml_diff>